<commit_message>
rework even more fields
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/heimathafen/dataDictionary.xlsx
+++ b/dataland-framework-toolbox/inputs/heimathafen/dataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\heimathafen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7DF5F9-4555-4CC6-BCF7-4D8FEF5B5051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E030086-7EBF-44EE-9FDD-398209F3809B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="328">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1108,6 +1108,9 @@
   <si>
     <t>Welche Quellen werden genutzt?
 Angabe von Quellen zur Erhebung der KPIs, zum Beispiel Umweltbundesamt.</t>
+  </si>
+  <si>
+    <t>Quellen</t>
   </si>
 </sst>
 </file>
@@ -1774,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA20BB-8F3E-44CB-A7F2-F957706EDEE9}">
   <dimension ref="A1:L1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2867,7 +2870,7 @@
         <v>75</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>85</v>
+        <v>327</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>86</v>

</xml_diff>